<commit_message>
Added Nodes to Distance Dataset (miles)
-Cougar Village Student Apartments
-Parc at 720 Student Apartments
-The Social Student Apartments
-Enclave Student Apartments
-The Reserves Student Apartments
</commit_message>
<xml_diff>
--- a/DataSet/Algorithms Data.xlsx
+++ b/DataSet/Algorithms Data.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECA9CC58-1636-4E9C-83EF-61F3DF035322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/logannitzsche/Documents/GitHub/Intelligent-Routing-for-Emergency-Services-in-Edwardsville/DataSet/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC9AFE0-5D22-EE40-89C3-733FE40C801A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="14800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>LOCATIONS</t>
   </si>
@@ -99,23 +104,53 @@
     <t>NOTE:</t>
   </si>
   <si>
-    <t>Minutes Distance Table Begins on BA9</t>
-  </si>
-  <si>
-    <t>Miles Distance Table Begins on G10</t>
-  </si>
-  <si>
     <t>Location Annotations and Node Coordinates Begins on A1</t>
   </si>
   <si>
-    <t>No Residential Areas Listed (Use API's, Coordinates, and User-provided Address to Calculate Distance)</t>
+    <t>(NO RESIDENTIAL AREAS)</t>
+  </si>
+  <si>
+    <t>Reserves Student Apartments = RA (38.80518785768586, -90.00950273315568)</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Parc at 720 Student Apartments = PA (38.80370049072766, -90.0118599711942)</t>
+  </si>
+  <si>
+    <t>Minutes Distance Table Begins on BA9 (no residential areas)</t>
+  </si>
+  <si>
+    <t>Miles Distance Table Begins on G10 (with residential areas)</t>
+  </si>
+  <si>
+    <t>The Social Student Apartments = SA (38.78475200026057, -89.98201421937024)</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>CVA</t>
+  </si>
+  <si>
+    <t>Cougar Village Apartments = CVA (38.80438098482753, -89.99518772883548)</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>Enclave Student Apartments = EA (38.80546832836268, -89.97140624030128)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,23 +522,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ22"/>
+  <dimension ref="A1:BJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:62">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -511,42 +546,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:62">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:62">
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:62">
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:62">
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:62">
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:62">
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:62">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.2">
       <c r="BA9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:62">
+      <c r="BB9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
         <v>9</v>
       </c>
@@ -577,6 +630,21 @@
       <c r="Q10" t="s">
         <v>18</v>
       </c>
+      <c r="R10" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" t="s">
+        <v>31</v>
+      </c>
+      <c r="V10" t="s">
+        <v>34</v>
+      </c>
       <c r="BA10" t="s">
         <v>19</v>
       </c>
@@ -605,7 +673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:62">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.2">
       <c r="I11" t="s">
         <v>11</v>
       </c>
@@ -633,6 +701,21 @@
       <c r="Q11">
         <v>5.5</v>
       </c>
+      <c r="R11">
+        <v>2.1</v>
+      </c>
+      <c r="S11">
+        <v>1.2</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>3.1</v>
+      </c>
+      <c r="V11">
+        <v>3.1</v>
+      </c>
       <c r="BB11" t="s">
         <v>11</v>
       </c>
@@ -661,7 +744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:62">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
         <v>12</v>
       </c>
@@ -689,6 +772,21 @@
       <c r="Q12">
         <v>3.4</v>
       </c>
+      <c r="R12">
+        <v>2.8</v>
+      </c>
+      <c r="S12">
+        <v>3.5</v>
+      </c>
+      <c r="T12">
+        <v>3.7</v>
+      </c>
+      <c r="U12">
+        <v>2.8</v>
+      </c>
+      <c r="V12">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="BB12" t="s">
         <v>12</v>
       </c>
@@ -717,7 +815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:62">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.2">
       <c r="I13" t="s">
         <v>20</v>
       </c>
@@ -745,6 +843,21 @@
       <c r="Q13">
         <v>2.1</v>
       </c>
+      <c r="R13">
+        <v>4.5</v>
+      </c>
+      <c r="S13">
+        <v>6.3</v>
+      </c>
+      <c r="T13">
+        <v>6.5</v>
+      </c>
+      <c r="U13">
+        <v>3.8</v>
+      </c>
+      <c r="V13">
+        <v>4.3</v>
+      </c>
       <c r="BB13" t="s">
         <v>13</v>
       </c>
@@ -773,7 +886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:62">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
         <v>14</v>
       </c>
@@ -801,6 +914,21 @@
       <c r="Q14">
         <v>5.4</v>
       </c>
+      <c r="R14">
+        <v>1.9</v>
+      </c>
+      <c r="S14">
+        <v>0.6</v>
+      </c>
+      <c r="T14">
+        <v>0.4</v>
+      </c>
+      <c r="U14">
+        <v>3</v>
+      </c>
+      <c r="V14">
+        <v>3</v>
+      </c>
       <c r="BB14" t="s">
         <v>14</v>
       </c>
@@ -829,7 +957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:62">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>15</v>
       </c>
@@ -857,6 +985,21 @@
       <c r="Q15">
         <v>3.4</v>
       </c>
+      <c r="R15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="S15">
+        <v>3.5</v>
+      </c>
+      <c r="T15">
+        <v>3.7</v>
+      </c>
+      <c r="U15">
+        <v>2.8</v>
+      </c>
+      <c r="V15">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="BB15" t="s">
         <v>15</v>
       </c>
@@ -885,7 +1028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:62">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
         <v>16</v>
       </c>
@@ -913,6 +1056,21 @@
       <c r="Q16">
         <v>4.5</v>
       </c>
+      <c r="R16">
+        <v>3.7</v>
+      </c>
+      <c r="S16">
+        <v>3.2</v>
+      </c>
+      <c r="T16">
+        <v>3.4</v>
+      </c>
+      <c r="U16">
+        <v>2.8</v>
+      </c>
+      <c r="V16">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="BB16" t="s">
         <v>16</v>
       </c>
@@ -941,7 +1099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:62">
+    <row r="17" spans="1:62" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
         <v>17</v>
       </c>
@@ -969,6 +1127,21 @@
       <c r="Q17">
         <v>5</v>
       </c>
+      <c r="R17">
+        <v>1.9</v>
+      </c>
+      <c r="S17">
+        <v>2.5</v>
+      </c>
+      <c r="T17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U17">
+        <v>2.4</v>
+      </c>
+      <c r="V17">
+        <v>2.6</v>
+      </c>
       <c r="BB17" t="s">
         <v>17</v>
       </c>
@@ -997,7 +1170,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:62">
+    <row r="18" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
       <c r="I18" t="s">
         <v>18</v>
       </c>
@@ -1025,6 +1204,21 @@
       <c r="Q18">
         <v>0</v>
       </c>
+      <c r="R18">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="S18">
+        <v>6.3</v>
+      </c>
+      <c r="T18">
+        <v>6.5</v>
+      </c>
+      <c r="U18">
+        <v>3.7</v>
+      </c>
+      <c r="V18">
+        <v>4.3</v>
+      </c>
       <c r="BB18" t="s">
         <v>18</v>
       </c>
@@ -1053,27 +1247,230 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:62">
+    <row r="19" spans="1:62" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19">
+        <v>2.1</v>
+      </c>
+      <c r="K19">
+        <v>2.8</v>
+      </c>
+      <c r="L19">
+        <v>4.5</v>
+      </c>
+      <c r="M19">
+        <v>1.9</v>
+      </c>
+      <c r="N19">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O19">
+        <v>3.7</v>
+      </c>
+      <c r="P19">
+        <v>1.9</v>
+      </c>
+      <c r="Q19">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>2.5</v>
+      </c>
+      <c r="T19">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V19">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="2:62">
-      <c r="C20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:62">
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:62">
-      <c r="C22" t="s">
+      <c r="I20" t="s">
         <v>25</v>
+      </c>
+      <c r="J20">
+        <v>1.2</v>
+      </c>
+      <c r="K20">
+        <v>3.5</v>
+      </c>
+      <c r="L20">
+        <v>6.3</v>
+      </c>
+      <c r="M20">
+        <v>0.6</v>
+      </c>
+      <c r="N20">
+        <v>3.5</v>
+      </c>
+      <c r="O20">
+        <v>3.2</v>
+      </c>
+      <c r="P20">
+        <v>2.5</v>
+      </c>
+      <c r="Q20">
+        <v>6.3</v>
+      </c>
+      <c r="R20">
+        <v>2.5</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0.2</v>
+      </c>
+      <c r="U20">
+        <v>4</v>
+      </c>
+      <c r="V20">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>3.7</v>
+      </c>
+      <c r="L21">
+        <v>6.5</v>
+      </c>
+      <c r="M21">
+        <v>0.4</v>
+      </c>
+      <c r="N21">
+        <v>3.7</v>
+      </c>
+      <c r="O21">
+        <v>3.4</v>
+      </c>
+      <c r="P21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q21">
+        <v>6.5</v>
+      </c>
+      <c r="R21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S21">
+        <v>0.2</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="V21">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22">
+        <v>3.1</v>
+      </c>
+      <c r="K22">
+        <v>2.8</v>
+      </c>
+      <c r="L22">
+        <v>3.8</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>2.8</v>
+      </c>
+      <c r="O22">
+        <v>2.8</v>
+      </c>
+      <c r="P22">
+        <v>2.4</v>
+      </c>
+      <c r="Q22">
+        <v>3.7</v>
+      </c>
+      <c r="R22">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S22">
+        <v>4</v>
+      </c>
+      <c r="T22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J23">
+        <v>3.1</v>
+      </c>
+      <c r="K23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L23">
+        <v>4.3</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P23">
+        <v>2.6</v>
+      </c>
+      <c r="Q23">
+        <v>4.3</v>
+      </c>
+      <c r="R23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S23">
+        <v>3.5</v>
+      </c>
+      <c r="T23">
+        <v>3.3</v>
+      </c>
+      <c r="U23">
+        <v>2</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>